<commit_message>
Review on Jul 3rd
</commit_message>
<xml_diff>
--- a/Crawling/files/youtube_rank.xlsx
+++ b/Crawling/files/youtube_rank.xlsx
@@ -3421,12 +3421,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>19억3964만</t>
+          <t>19억4131만</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>1,439개</t>
+          <t>1,441개</t>
         </is>
       </c>
     </row>
@@ -3865,34 +3865,34 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>KBS Drama</t>
+          <t>소맥거핀</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[게임]</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>389만</t>
+          <t>390만</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>53억3598만</t>
+          <t>15억4061만</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>131,317개</t>
+          <t>312개</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>워크맨-Workman</t>
+          <t>KBS Drama</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3902,56 +3902,56 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>388만</t>
+          <t>389만</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>10억4849만</t>
+          <t>53억3598만</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>284개</t>
+          <t>131,317개</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>English Singsing</t>
+          <t>워크맨-Workman</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>[키즈/어린이]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>387만</t>
+          <t>388만</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>8억5551만</t>
+          <t>10억4849만</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>1,266개</t>
+          <t>284개</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>소맥거핀</t>
+          <t>English Singsing</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>[게임]</t>
+          <t>[키즈/어린이]</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3961,12 +3961,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>15억2884만</t>
+          <t>8억5551만</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>311개</t>
+          <t>1,266개</t>
         </is>
       </c>
     </row>
@@ -4496,12 +4496,12 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>358만</t>
+          <t>359만</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>18억7401만</t>
+          <t>18억7669만</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -5036,12 +5036,12 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>325만</t>
+          <t>324만</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>27억2963만</t>
+          <t>27억2981만</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -6079,39 +6079,39 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>쿠킹하루 Cooking Haru :)</t>
+          <t>짤툰</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[영화/만화/애니]</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>262만</t>
+          <t>263만</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>3억2507만</t>
+          <t>21억7372만</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>183개</t>
+          <t>1,391개</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>짤툰</t>
+          <t>쿠킹하루 Cooking Haru :)</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>[영화/만화/애니]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -6121,12 +6121,12 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>21억6542만</t>
+          <t>3억2507만</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>1,383개</t>
+          <t>183개</t>
         </is>
       </c>
     </row>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>4982만</t>
+          <t>4983만</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
@@ -6700,39 +6700,39 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>뽀송한 준_bosungjun</t>
+          <t>ITSub잇섭</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[IT/기술/컴퓨터]</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>237만</t>
+          <t>238만</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>2억5368만</t>
+          <t>9억4464만</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>369개</t>
+          <t>1,073개</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>KBS News</t>
+          <t>뽀송한 준_bosungjun</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>[뉴스/정치/사회]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -6742,24 +6742,24 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>50억5373만</t>
+          <t>2억5368만</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>257,539개</t>
+          <t>369개</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>ToytubeTV 토이튜브TV</t>
+          <t>KBS News</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>[키즈/어린이]</t>
+          <t>[뉴스/정치/사회]</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -6769,24 +6769,24 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>2억8981만</t>
+          <t>50억5373만</t>
         </is>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>51개</t>
+          <t>257,539개</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>ITSub잇섭</t>
+          <t>ToytubeTV 토이튜브TV</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>[IT/기술/컴퓨터]</t>
+          <t>[키즈/어린이]</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -6796,12 +6796,12 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>9억4302만</t>
+          <t>2억8981만</t>
         </is>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>1,072개</t>
+          <t>51개</t>
         </is>
       </c>
     </row>
@@ -6850,7 +6850,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>27억9398만</t>
+          <t>27억9449만</t>
         </is>
       </c>
       <c r="E238" t="inlineStr">
@@ -6958,7 +6958,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>3억1047만</t>
+          <t>3억1059만</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>2억1065만</t>
+          <t>2억1078만</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
@@ -7795,7 +7795,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>6억7930만</t>
+          <t>6억8037만</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -7871,12 +7871,12 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>215만</t>
+          <t>216만</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>9억2923만</t>
+          <t>9억3232만</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -7888,39 +7888,39 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>[THE SOY]루퐁이네</t>
+          <t>올리버쌤</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>[애완/반려동물]</t>
+          <t>[교육/강의]</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>214만</t>
+          <t>215만</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>8억4743만</t>
+          <t>7억9162만</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>551개</t>
+          <t>846개</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>4Minute 포미닛(Official YouTube Channel)</t>
+          <t>[THE SOY]루퐁이네</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>[음악/댄스/가수]</t>
+          <t>[애완/반려동물]</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -7930,24 +7930,24 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>13억8606만</t>
+          <t>8억4743만</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>82개</t>
+          <t>551개</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>올리버쌤</t>
+          <t>4Minute 포미닛(Official YouTube Channel)</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>[교육/강의]</t>
+          <t>[음악/댄스/가수]</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -7957,12 +7957,12 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>7억9068만</t>
+          <t>13억8606만</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>846개</t>
+          <t>82개</t>
         </is>
       </c>
     </row>
@@ -8941,12 +8941,12 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>ARIRANG K-POP</t>
+          <t>Jung Kook - Topic</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>[음악/댄스/가수]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -8956,24 +8956,24 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>8억8085만</t>
+          <t>8186만</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>32,834개</t>
+          <t>5개</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Dollightful</t>
+          <t>ARIRANG K-POP</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>[키즈/어린이]</t>
+          <t>[음악/댄스/가수]</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -8983,19 +8983,19 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>3억2316만</t>
+          <t>8억8085만</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>168개</t>
+          <t>32,834개</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>대문밖장덕대</t>
+          <t>Dollightful</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -9010,39 +9010,39 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>9억3725만</t>
+          <t>3억2316만</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>1,650개</t>
+          <t>168개</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Jung Kook - Topic</t>
+          <t>대문밖장덕대</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[키즈/어린이]</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>195만</t>
+          <t>196만</t>
         </is>
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>8148만</t>
+          <t>9억3725만</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>3개</t>
+          <t>1,650개</t>
         </is>
       </c>
     </row>
@@ -9280,12 +9280,12 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>5억6236만</t>
+          <t>5억6414만</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>442개</t>
+          <t>444개</t>
         </is>
       </c>
     </row>
@@ -9388,12 +9388,12 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>8억7701만</t>
+          <t>8억7704만</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>895개</t>
+          <t>896개</t>
         </is>
       </c>
     </row>
@@ -10333,12 +10333,12 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>13억4888만</t>
+          <t>13억5145만</t>
         </is>
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>1,344개</t>
+          <t>1,349개</t>
         </is>
       </c>
     </row>
@@ -10603,12 +10603,12 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>12억1762만</t>
+          <t>12억2021만</t>
         </is>
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>2,353개</t>
+          <t>2,356개</t>
         </is>
       </c>
     </row>
@@ -11479,12 +11479,12 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>파뿌리</t>
+          <t>김대석 셰프TV</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>[음식/요리/레시피]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
@@ -11494,39 +11494,39 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>18억5936만</t>
+          <t>3억2425만</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>1,723개</t>
+          <t>829개</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>김대석 셰프TV</t>
+          <t>파뿌리</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[음식/요리/레시피]</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>156만</t>
+          <t>157만</t>
         </is>
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>3억2235만</t>
+          <t>18억5936만</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>825개</t>
+          <t>1,723개</t>
         </is>
       </c>
     </row>
@@ -11818,12 +11818,12 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>8억5469만</t>
+          <t>8억5583만</t>
         </is>
       </c>
       <c r="E422" t="inlineStr">
         <is>
-          <t>1,783개</t>
+          <t>1,784개</t>
         </is>
       </c>
     </row>
@@ -11926,12 +11926,12 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>21억6633만</t>
+          <t>21억6987만</t>
         </is>
       </c>
       <c r="E426" t="inlineStr">
         <is>
-          <t>62,343개</t>
+          <t>62,347개</t>
         </is>
       </c>
     </row>
@@ -12034,12 +12034,12 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>4억1348만</t>
+          <t>4억1382만</t>
         </is>
       </c>
       <c r="E430" t="inlineStr">
         <is>
-          <t>745개</t>
+          <t>746개</t>
         </is>
       </c>
     </row>
@@ -12115,7 +12115,7 @@
       </c>
       <c r="D433" t="inlineStr">
         <is>
-          <t>6억4233만</t>
+          <t>6억4239만</t>
         </is>
       </c>
       <c r="E433" t="inlineStr">
@@ -12385,12 +12385,12 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>2억9586만</t>
+          <t>2억9890만</t>
         </is>
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t>223개</t>
+          <t>224개</t>
         </is>
       </c>
     </row>
@@ -12817,12 +12817,12 @@
       </c>
       <c r="D459" t="inlineStr">
         <is>
-          <t>4억6086만</t>
+          <t>4억6240만</t>
         </is>
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t>509개</t>
+          <t>510개</t>
         </is>
       </c>
     </row>
@@ -12979,12 +12979,12 @@
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>7억8765만</t>
+          <t>7억8860만</t>
         </is>
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>9,331개</t>
+          <t>9,353개</t>
         </is>
       </c>
     </row>
@@ -13423,12 +13423,12 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>달라스튜디오</t>
+          <t>FIFTY FIFTY Official</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
@@ -13438,19 +13438,19 @@
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>3억8656만</t>
+          <t>3억3537만</t>
         </is>
       </c>
       <c r="E482" t="inlineStr">
         <is>
-          <t>276개</t>
+          <t>100개</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>KBS CoolFM</t>
+          <t>달라스튜디오</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
@@ -13465,24 +13465,24 @@
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>7억4841만</t>
+          <t>3억8656만</t>
         </is>
       </c>
       <c r="E483" t="inlineStr">
         <is>
-          <t>12,701개</t>
+          <t>276개</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>BEAST 비스트 (Official YouTube Channel)</t>
+          <t>KBS CoolFM</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>[음악/댄스/가수]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
@@ -13492,39 +13492,39 @@
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>6억2607만</t>
+          <t>7억4841만</t>
         </is>
       </c>
       <c r="E484" t="inlineStr">
         <is>
-          <t>118개</t>
+          <t>12,701개</t>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>FIFTY FIFTY Official</t>
+          <t>BEAST 비스트 (Official YouTube Channel)</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[음악/댄스/가수]</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>136만</t>
+          <t>137만</t>
         </is>
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>3억2894만</t>
+          <t>6억2607만</t>
         </is>
       </c>
       <c r="E485" t="inlineStr">
         <is>
-          <t>100개</t>
+          <t>118개</t>
         </is>
       </c>
     </row>
@@ -13978,12 +13978,12 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>10억6117만</t>
+          <t>10억6484만</t>
         </is>
       </c>
       <c r="E502" t="inlineStr">
         <is>
-          <t>16,854개</t>
+          <t>16,872개</t>
         </is>
       </c>
     </row>
@@ -14356,12 +14356,12 @@
       </c>
       <c r="D516" t="inlineStr">
         <is>
-          <t>22억2466만</t>
+          <t>22억2721만</t>
         </is>
       </c>
       <c r="E516" t="inlineStr">
         <is>
-          <t>7,164개</t>
+          <t>7,171개</t>
         </is>
       </c>
     </row>
@@ -14410,12 +14410,12 @@
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>6억8740만</t>
+          <t>6억8849만</t>
         </is>
       </c>
       <c r="E518" t="inlineStr">
         <is>
-          <t>29,772개</t>
+          <t>29,787개</t>
         </is>
       </c>
     </row>
@@ -14653,7 +14653,7 @@
       </c>
       <c r="D527" t="inlineStr">
         <is>
-          <t>3억3010만</t>
+          <t>3억3013만</t>
         </is>
       </c>
       <c r="E527" t="inlineStr">
@@ -14923,7 +14923,7 @@
       </c>
       <c r="D537" t="inlineStr">
         <is>
-          <t>6249만</t>
+          <t>6254만</t>
         </is>
       </c>
       <c r="E537" t="inlineStr">
@@ -15139,12 +15139,12 @@
       </c>
       <c r="D545" t="inlineStr">
         <is>
-          <t>1억0893만</t>
+          <t>1억0900만</t>
         </is>
       </c>
       <c r="E545" t="inlineStr">
         <is>
-          <t>534개</t>
+          <t>536개</t>
         </is>
       </c>
     </row>
@@ -15220,12 +15220,12 @@
       </c>
       <c r="D548" t="inlineStr">
         <is>
-          <t>1억1225만</t>
+          <t>1억1300만</t>
         </is>
       </c>
       <c r="E548" t="inlineStr">
         <is>
-          <t>477개</t>
+          <t>478개</t>
         </is>
       </c>
     </row>
@@ -15490,12 +15490,12 @@
       </c>
       <c r="D558" t="inlineStr">
         <is>
-          <t>1억4122만</t>
+          <t>1억4167만</t>
         </is>
       </c>
       <c r="E558" t="inlineStr">
         <is>
-          <t>87개</t>
+          <t>88개</t>
         </is>
       </c>
     </row>
@@ -15922,7 +15922,7 @@
       </c>
       <c r="D574" t="inlineStr">
         <is>
-          <t>3억3541만</t>
+          <t>3억3559만</t>
         </is>
       </c>
       <c r="E574" t="inlineStr">
@@ -16111,12 +16111,12 @@
       </c>
       <c r="D581" t="inlineStr">
         <is>
-          <t>2억2996만</t>
+          <t>2억3019만</t>
         </is>
       </c>
       <c r="E581" t="inlineStr">
         <is>
-          <t>625개</t>
+          <t>626개</t>
         </is>
       </c>
     </row>
@@ -16624,12 +16624,12 @@
       </c>
       <c r="D600" t="inlineStr">
         <is>
-          <t>2억5886만</t>
+          <t>2억5998만</t>
         </is>
       </c>
       <c r="E600" t="inlineStr">
         <is>
-          <t>357개</t>
+          <t>359개</t>
         </is>
       </c>
     </row>
@@ -16717,12 +16717,12 @@
     <row r="604">
       <c r="A604" t="inlineStr">
         <is>
-          <t>SK telecom</t>
+          <t>DAZBEE official</t>
         </is>
       </c>
       <c r="B604" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[영화/만화/애니]</t>
         </is>
       </c>
       <c r="C604" t="inlineStr">
@@ -16732,24 +16732,24 @@
       </c>
       <c r="D604" t="inlineStr">
         <is>
-          <t>9억8441만</t>
+          <t>5억0480만</t>
         </is>
       </c>
       <c r="E604" t="inlineStr">
         <is>
-          <t>2,397개</t>
+          <t>182개</t>
         </is>
       </c>
     </row>
     <row r="605">
       <c r="A605" t="inlineStr">
         <is>
-          <t>퍼플 토이박스(Purple Toy Box)</t>
+          <t>SK telecom</t>
         </is>
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>[키즈/어린이]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C605" t="inlineStr">
@@ -16759,24 +16759,24 @@
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>7억1217만</t>
+          <t>9억8441만</t>
         </is>
       </c>
       <c r="E605" t="inlineStr">
         <is>
-          <t>1,459개</t>
+          <t>2,397개</t>
         </is>
       </c>
     </row>
     <row r="606">
       <c r="A606" t="inlineStr">
         <is>
-          <t>다또아Daddoa</t>
+          <t>퍼플 토이박스(Purple Toy Box)</t>
         </is>
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>[패션/미용]</t>
+          <t>[키즈/어린이]</t>
         </is>
       </c>
       <c r="C606" t="inlineStr">
@@ -16786,24 +16786,24 @@
       </c>
       <c r="D606" t="inlineStr">
         <is>
-          <t>9436만</t>
+          <t>7억1217만</t>
         </is>
       </c>
       <c r="E606" t="inlineStr">
         <is>
-          <t>190개</t>
+          <t>1,459개</t>
         </is>
       </c>
     </row>
     <row r="607">
       <c r="A607" t="inlineStr">
         <is>
-          <t>야식이</t>
+          <t>다또아Daddoa</t>
         </is>
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>[음식/요리/레시피]</t>
+          <t>[패션/미용]</t>
         </is>
       </c>
       <c r="C607" t="inlineStr">
@@ -16813,19 +16813,19 @@
       </c>
       <c r="D607" t="inlineStr">
         <is>
-          <t>4억6273만</t>
+          <t>9436만</t>
         </is>
       </c>
       <c r="E607" t="inlineStr">
         <is>
-          <t>1,475개</t>
+          <t>190개</t>
         </is>
       </c>
     </row>
     <row r="608">
       <c r="A608" t="inlineStr">
         <is>
-          <t>애주가TV참PD</t>
+          <t>야식이</t>
         </is>
       </c>
       <c r="B608" t="inlineStr">
@@ -16840,51 +16840,51 @@
       </c>
       <c r="D608" t="inlineStr">
         <is>
-          <t>6억3305만</t>
+          <t>4억6273만</t>
         </is>
       </c>
       <c r="E608" t="inlineStr">
         <is>
-          <t>1,357개</t>
+          <t>1,475개</t>
         </is>
       </c>
     </row>
     <row r="609">
       <c r="A609" t="inlineStr">
         <is>
-          <t>할명수</t>
+          <t>애주가TV참PD</t>
         </is>
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[음식/요리/레시피]</t>
         </is>
       </c>
       <c r="C609" t="inlineStr">
         <is>
-          <t>114만</t>
+          <t>115만</t>
         </is>
       </c>
       <c r="D609" t="inlineStr">
         <is>
-          <t>2억4056만</t>
+          <t>6억3305만</t>
         </is>
       </c>
       <c r="E609" t="inlineStr">
         <is>
-          <t>296개</t>
+          <t>1,357개</t>
         </is>
       </c>
     </row>
     <row r="610">
       <c r="A610" t="inlineStr">
         <is>
-          <t>Variety</t>
+          <t>할명수</t>
         </is>
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>[해외]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C610" t="inlineStr">
@@ -16894,24 +16894,24 @@
       </c>
       <c r="D610" t="inlineStr">
         <is>
-          <t>5억2319만</t>
+          <t>2억4056만</t>
         </is>
       </c>
       <c r="E610" t="inlineStr">
         <is>
-          <t>5,160개</t>
+          <t>296개</t>
         </is>
       </c>
     </row>
     <row r="611">
       <c r="A611" t="inlineStr">
         <is>
-          <t>올끌 (All of MBClassic)</t>
+          <t>Variety</t>
         </is>
       </c>
       <c r="B611" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[해외]</t>
         </is>
       </c>
       <c r="C611" t="inlineStr">
@@ -16921,24 +16921,24 @@
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>20억3925만</t>
+          <t>5억2319만</t>
         </is>
       </c>
       <c r="E611" t="inlineStr">
         <is>
-          <t>3,365개</t>
+          <t>5,160개</t>
         </is>
       </c>
     </row>
     <row r="612">
       <c r="A612" t="inlineStr">
         <is>
-          <t>DAZBEE official</t>
+          <t>올끌 (All of MBClassic)</t>
         </is>
       </c>
       <c r="B612" t="inlineStr">
         <is>
-          <t>[영화/만화/애니]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C612" t="inlineStr">
@@ -16948,12 +16948,12 @@
       </c>
       <c r="D612" t="inlineStr">
         <is>
-          <t>5억0334만</t>
+          <t>20억3925만</t>
         </is>
       </c>
       <c r="E612" t="inlineStr">
         <is>
-          <t>182개</t>
+          <t>3,365개</t>
         </is>
       </c>
     </row>
@@ -16975,12 +16975,12 @@
       </c>
       <c r="D613" t="inlineStr">
         <is>
-          <t>5억0547만</t>
+          <t>5억0568만</t>
         </is>
       </c>
       <c r="E613" t="inlineStr">
         <is>
-          <t>811개</t>
+          <t>812개</t>
         </is>
       </c>
     </row>
@@ -17095,12 +17095,12 @@
     <row r="618">
       <c r="A618" t="inlineStr">
         <is>
-          <t>강다니엘 KANGDANIEL</t>
+          <t>랄랄ralral</t>
         </is>
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>[음악/댄스/가수]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C618" t="inlineStr">
@@ -17110,24 +17110,24 @@
       </c>
       <c r="D618" t="inlineStr">
         <is>
-          <t>2억1502만</t>
+          <t>4억3718만</t>
         </is>
       </c>
       <c r="E618" t="inlineStr">
         <is>
-          <t>205개</t>
+          <t>718개</t>
         </is>
       </c>
     </row>
     <row r="619">
       <c r="A619" t="inlineStr">
         <is>
-          <t>Bravo jamoasi</t>
+          <t>강다니엘 KANGDANIEL</t>
         </is>
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[음악/댄스/가수]</t>
         </is>
       </c>
       <c r="C619" t="inlineStr">
@@ -17137,24 +17137,24 @@
       </c>
       <c r="D619" t="inlineStr">
         <is>
-          <t>2억7552만</t>
+          <t>2억1502만</t>
         </is>
       </c>
       <c r="E619" t="inlineStr">
         <is>
-          <t>142개</t>
+          <t>205개</t>
         </is>
       </c>
     </row>
     <row r="620">
       <c r="A620" t="inlineStr">
         <is>
-          <t>CLC 씨엘씨 (Official YouTube Channel)</t>
+          <t>Bravo jamoasi</t>
         </is>
       </c>
       <c r="B620" t="inlineStr">
         <is>
-          <t>[음악/댄스/가수]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C620" t="inlineStr">
@@ -17164,24 +17164,24 @@
       </c>
       <c r="D620" t="inlineStr">
         <is>
-          <t>2억7860만</t>
+          <t>2억7617만</t>
         </is>
       </c>
       <c r="E620" t="inlineStr">
         <is>
-          <t>188개</t>
+          <t>142개</t>
         </is>
       </c>
     </row>
     <row r="621">
       <c r="A621" t="inlineStr">
         <is>
-          <t>Godtuk 턱형</t>
+          <t>CLC 씨엘씨 (Official YouTube Channel)</t>
         </is>
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>[BJ/인물/연예인]</t>
+          <t>[음악/댄스/가수]</t>
         </is>
       </c>
       <c r="C621" t="inlineStr">
@@ -17191,24 +17191,24 @@
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>4억2532만</t>
+          <t>2억7876만</t>
         </is>
       </c>
       <c r="E621" t="inlineStr">
         <is>
-          <t>507개</t>
+          <t>188개</t>
         </is>
       </c>
     </row>
     <row r="622">
       <c r="A622" t="inlineStr">
         <is>
-          <t>드림텔러(DreamTeller)</t>
+          <t>Godtuk 턱형</t>
         </is>
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>[영화/만화/애니]</t>
+          <t>[BJ/인물/연예인]</t>
         </is>
       </c>
       <c r="C622" t="inlineStr">
@@ -17218,24 +17218,24 @@
       </c>
       <c r="D622" t="inlineStr">
         <is>
-          <t>1억9865만</t>
+          <t>4억2532만</t>
         </is>
       </c>
       <c r="E622" t="inlineStr">
         <is>
-          <t>197개</t>
+          <t>507개</t>
         </is>
       </c>
     </row>
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>[팟빵] 매불쇼</t>
+          <t>드림텔러(DreamTeller)</t>
         </is>
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>[뉴스/정치/사회]</t>
+          <t>[영화/만화/애니]</t>
         </is>
       </c>
       <c r="C623" t="inlineStr">
@@ -17245,39 +17245,39 @@
       </c>
       <c r="D623" t="inlineStr">
         <is>
-          <t>5억4292만</t>
+          <t>1억9865만</t>
         </is>
       </c>
       <c r="E623" t="inlineStr">
         <is>
-          <t>1,532개</t>
+          <t>197개</t>
         </is>
       </c>
     </row>
     <row r="624">
       <c r="A624" t="inlineStr">
         <is>
-          <t>랄랄ralral</t>
+          <t>[팟빵] 매불쇼</t>
         </is>
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[뉴스/정치/사회]</t>
         </is>
       </c>
       <c r="C624" t="inlineStr">
         <is>
-          <t>112만</t>
+          <t>113만</t>
         </is>
       </c>
       <c r="D624" t="inlineStr">
         <is>
-          <t>4억3266만</t>
+          <t>5억4292만</t>
         </is>
       </c>
       <c r="E624" t="inlineStr">
         <is>
-          <t>714개</t>
+          <t>1,532개</t>
         </is>
       </c>
     </row>
@@ -17353,7 +17353,7 @@
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>5억4851만</t>
+          <t>5억4894만</t>
         </is>
       </c>
       <c r="E627" t="inlineStr">
@@ -17650,7 +17650,7 @@
       </c>
       <c r="D638" t="inlineStr">
         <is>
-          <t>1억9107만</t>
+          <t>1억9109만</t>
         </is>
       </c>
       <c r="E638" t="inlineStr">
@@ -17812,12 +17812,12 @@
       </c>
       <c r="D644" t="inlineStr">
         <is>
-          <t>7억4473만</t>
+          <t>7억4777만</t>
         </is>
       </c>
       <c r="E644" t="inlineStr">
         <is>
-          <t>14,701개</t>
+          <t>14,725개</t>
         </is>
       </c>
     </row>
@@ -17947,7 +17947,7 @@
       </c>
       <c r="D649" t="inlineStr">
         <is>
-          <t>2억7236만</t>
+          <t>2억7243만</t>
         </is>
       </c>
       <c r="E649" t="inlineStr">
@@ -18487,12 +18487,12 @@
       </c>
       <c r="D669" t="inlineStr">
         <is>
-          <t>9억3454만</t>
+          <t>9억3809만</t>
         </is>
       </c>
       <c r="E669" t="inlineStr">
         <is>
-          <t>16,477개</t>
+          <t>16,541개</t>
         </is>
       </c>
     </row>
@@ -19378,12 +19378,12 @@
       </c>
       <c r="D702" t="inlineStr">
         <is>
-          <t>7억7047만</t>
+          <t>7억7316만</t>
         </is>
       </c>
       <c r="E702" t="inlineStr">
         <is>
-          <t>3,529개</t>
+          <t>3,544개</t>
         </is>
       </c>
     </row>
@@ -19756,12 +19756,12 @@
       </c>
       <c r="D716" t="inlineStr">
         <is>
-          <t>9억7471만</t>
+          <t>9억7538만</t>
         </is>
       </c>
       <c r="E716" t="inlineStr">
         <is>
-          <t>2,809개</t>
+          <t>2,810개</t>
         </is>
       </c>
     </row>
@@ -19849,7 +19849,7 @@
     <row r="720">
       <c r="A720" t="inlineStr">
         <is>
-          <t>이재성 박사의 식탁보감</t>
+          <t>셜록현준</t>
         </is>
       </c>
       <c r="B720" t="inlineStr">
@@ -19864,19 +19864,19 @@
       </c>
       <c r="D720" t="inlineStr">
         <is>
-          <t>1억1210만</t>
+          <t>8906만</t>
         </is>
       </c>
       <c r="E720" t="inlineStr">
         <is>
-          <t>382개</t>
+          <t>145개</t>
         </is>
       </c>
     </row>
     <row r="721">
       <c r="A721" t="inlineStr">
         <is>
-          <t>정찬성 Korean Zombie</t>
+          <t>이재성 박사의 식탁보감</t>
         </is>
       </c>
       <c r="B721" t="inlineStr">
@@ -19891,24 +19891,24 @@
       </c>
       <c r="D721" t="inlineStr">
         <is>
-          <t>3억2284만</t>
+          <t>1억1210만</t>
         </is>
       </c>
       <c r="E721" t="inlineStr">
         <is>
-          <t>312개</t>
+          <t>382개</t>
         </is>
       </c>
     </row>
     <row r="722">
       <c r="A722" t="inlineStr">
         <is>
-          <t>Robot Trains official</t>
+          <t>정찬성 Korean Zombie</t>
         </is>
       </c>
       <c r="B722" t="inlineStr">
         <is>
-          <t>[키즈/어린이]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C722" t="inlineStr">
@@ -19918,24 +19918,24 @@
       </c>
       <c r="D722" t="inlineStr">
         <is>
-          <t>7억6191만</t>
+          <t>3억2284만</t>
         </is>
       </c>
       <c r="E722" t="inlineStr">
         <is>
-          <t>744개</t>
+          <t>312개</t>
         </is>
       </c>
     </row>
     <row r="723">
       <c r="A723" t="inlineStr">
         <is>
-          <t>바바요 by iHQ</t>
+          <t>Robot Trains official</t>
         </is>
       </c>
       <c r="B723" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[키즈/어린이]</t>
         </is>
       </c>
       <c r="C723" t="inlineStr">
@@ -19945,24 +19945,24 @@
       </c>
       <c r="D723" t="inlineStr">
         <is>
-          <t>7억8453만</t>
+          <t>7억6191만</t>
         </is>
       </c>
       <c r="E723" t="inlineStr">
         <is>
-          <t>7,625개</t>
+          <t>744개</t>
         </is>
       </c>
     </row>
     <row r="724">
       <c r="A724" t="inlineStr">
         <is>
-          <t>친절한 대학</t>
+          <t>바바요 by iHQ</t>
         </is>
       </c>
       <c r="B724" t="inlineStr">
         <is>
-          <t>[교육/강의]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C724" t="inlineStr">
@@ -19972,24 +19972,24 @@
       </c>
       <c r="D724" t="inlineStr">
         <is>
-          <t>1억1088만</t>
+          <t>7억8453만</t>
         </is>
       </c>
       <c r="E724" t="inlineStr">
         <is>
-          <t>782개</t>
+          <t>7,625개</t>
         </is>
       </c>
     </row>
     <row r="725">
       <c r="A725" t="inlineStr">
         <is>
-          <t>맛있는 녀석들 (Tasty Guys)</t>
+          <t>친절한 대학</t>
         </is>
       </c>
       <c r="B725" t="inlineStr">
         <is>
-          <t>[음식/요리/레시피]</t>
+          <t>[교육/강의]</t>
         </is>
       </c>
       <c r="C725" t="inlineStr">
@@ -19999,24 +19999,24 @@
       </c>
       <c r="D725" t="inlineStr">
         <is>
-          <t>13억4991만</t>
+          <t>1억1088만</t>
         </is>
       </c>
       <c r="E725" t="inlineStr">
         <is>
-          <t>4,584개</t>
+          <t>782개</t>
         </is>
       </c>
     </row>
     <row r="726">
       <c r="A726" t="inlineStr">
         <is>
-          <t>말왕TV</t>
+          <t>맛있는 녀석들 (Tasty Guys)</t>
         </is>
       </c>
       <c r="B726" t="inlineStr">
         <is>
-          <t>[스포츠/운동]</t>
+          <t>[음식/요리/레시피]</t>
         </is>
       </c>
       <c r="C726" t="inlineStr">
@@ -20026,24 +20026,24 @@
       </c>
       <c r="D726" t="inlineStr">
         <is>
-          <t>4억0121만</t>
+          <t>13억4991만</t>
         </is>
       </c>
       <c r="E726" t="inlineStr">
         <is>
-          <t>1,012개</t>
+          <t>4,584개</t>
         </is>
       </c>
     </row>
     <row r="727">
       <c r="A727" t="inlineStr">
         <is>
-          <t>텔론</t>
+          <t>말왕TV</t>
         </is>
       </c>
       <c r="B727" t="inlineStr">
         <is>
-          <t>[게임]</t>
+          <t>[스포츠/운동]</t>
         </is>
       </c>
       <c r="C727" t="inlineStr">
@@ -20053,24 +20053,24 @@
       </c>
       <c r="D727" t="inlineStr">
         <is>
-          <t>11억5807만</t>
+          <t>4억0121만</t>
         </is>
       </c>
       <c r="E727" t="inlineStr">
         <is>
-          <t>4,367개</t>
+          <t>1,012개</t>
         </is>
       </c>
     </row>
     <row r="728">
       <c r="A728" t="inlineStr">
         <is>
-          <t>U.M.A.우마</t>
+          <t>텔론</t>
         </is>
       </c>
       <c r="B728" t="inlineStr">
         <is>
-          <t>[BJ/인물/연예인]</t>
+          <t>[게임]</t>
         </is>
       </c>
       <c r="C728" t="inlineStr">
@@ -20080,24 +20080,24 @@
       </c>
       <c r="D728" t="inlineStr">
         <is>
-          <t>2억7007만</t>
+          <t>11억5807만</t>
         </is>
       </c>
       <c r="E728" t="inlineStr">
         <is>
-          <t>147개</t>
+          <t>4,367개</t>
         </is>
       </c>
     </row>
     <row r="729">
       <c r="A729" t="inlineStr">
         <is>
-          <t>소녀의행성 Girlsplanet</t>
+          <t>U.M.A.우마</t>
         </is>
       </c>
       <c r="B729" t="inlineStr">
         <is>
-          <t>[애완/반려동물]</t>
+          <t>[BJ/인물/연예인]</t>
         </is>
       </c>
       <c r="C729" t="inlineStr">
@@ -20107,39 +20107,39 @@
       </c>
       <c r="D729" t="inlineStr">
         <is>
-          <t>4억1844만</t>
+          <t>2억7007만</t>
         </is>
       </c>
       <c r="E729" t="inlineStr">
         <is>
-          <t>576개</t>
+          <t>147개</t>
         </is>
       </c>
     </row>
     <row r="730">
       <c r="A730" t="inlineStr">
         <is>
-          <t>셜록현준</t>
+          <t>소녀의행성 Girlsplanet</t>
         </is>
       </c>
       <c r="B730" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[애완/반려동물]</t>
         </is>
       </c>
       <c r="C730" t="inlineStr">
         <is>
-          <t>100만</t>
+          <t>101만</t>
         </is>
       </c>
       <c r="D730" t="inlineStr">
         <is>
-          <t>8811만</t>
+          <t>4억1844만</t>
         </is>
       </c>
       <c r="E730" t="inlineStr">
         <is>
-          <t>143개</t>
+          <t>576개</t>
         </is>
       </c>
     </row>
@@ -20323,12 +20323,12 @@
       </c>
       <c r="D737" t="inlineStr">
         <is>
-          <t>3억2022만</t>
+          <t>3억2050만</t>
         </is>
       </c>
       <c r="E737" t="inlineStr">
         <is>
-          <t>2,867개</t>
+          <t>2,868개</t>
         </is>
       </c>
     </row>
@@ -20956,12 +20956,12 @@
     <row r="761">
       <c r="A761" t="inlineStr">
         <is>
-          <t>메리니즈부엌Meliniskitchen</t>
+          <t>어퍼컷Tube</t>
         </is>
       </c>
       <c r="B761" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[영화/만화/애니]</t>
         </is>
       </c>
       <c r="C761" t="inlineStr">
@@ -20971,24 +20971,24 @@
       </c>
       <c r="D761" t="inlineStr">
         <is>
-          <t>1억8660만</t>
+          <t>2억4274만</t>
         </is>
       </c>
       <c r="E761" t="inlineStr">
         <is>
-          <t>242개</t>
+          <t>258개</t>
         </is>
       </c>
     </row>
     <row r="762">
       <c r="A762" t="inlineStr">
         <is>
-          <t>범석TV</t>
+          <t>메리니즈부엌Meliniskitchen</t>
         </is>
       </c>
       <c r="B762" t="inlineStr">
         <is>
-          <t>[게임]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C762" t="inlineStr">
@@ -20998,19 +20998,19 @@
       </c>
       <c r="D762" t="inlineStr">
         <is>
-          <t>7억5591만</t>
+          <t>1억8660만</t>
         </is>
       </c>
       <c r="E762" t="inlineStr">
         <is>
-          <t>1,868개</t>
+          <t>242개</t>
         </is>
       </c>
     </row>
     <row r="763">
       <c r="A763" t="inlineStr">
         <is>
-          <t>GCL 지씨엘</t>
+          <t>범석TV</t>
         </is>
       </c>
       <c r="B763" t="inlineStr">
@@ -21020,29 +21020,29 @@
       </c>
       <c r="C763" t="inlineStr">
         <is>
-          <t>96만</t>
+          <t>97만</t>
         </is>
       </c>
       <c r="D763" t="inlineStr">
         <is>
-          <t>3억2475만</t>
+          <t>7억5591만</t>
         </is>
       </c>
       <c r="E763" t="inlineStr">
         <is>
-          <t>400개</t>
+          <t>1,868개</t>
         </is>
       </c>
     </row>
     <row r="764">
       <c r="A764" t="inlineStr">
         <is>
-          <t>어퍼컷Tube</t>
+          <t>GCL 지씨엘</t>
         </is>
       </c>
       <c r="B764" t="inlineStr">
         <is>
-          <t>[영화/만화/애니]</t>
+          <t>[게임]</t>
         </is>
       </c>
       <c r="C764" t="inlineStr">
@@ -21052,12 +21052,12 @@
       </c>
       <c r="D764" t="inlineStr">
         <is>
-          <t>2억4130만</t>
+          <t>3억2475만</t>
         </is>
       </c>
       <c r="E764" t="inlineStr">
         <is>
-          <t>257개</t>
+          <t>400개</t>
         </is>
       </c>
     </row>
@@ -21106,24 +21106,24 @@
       </c>
       <c r="D766" t="inlineStr">
         <is>
-          <t>23억5860만</t>
+          <t>23억6160만</t>
         </is>
       </c>
       <c r="E766" t="inlineStr">
         <is>
-          <t>2,659개</t>
+          <t>2,663개</t>
         </is>
       </c>
     </row>
     <row r="767">
       <c r="A767" t="inlineStr">
         <is>
-          <t>얌무YAMMoo</t>
+          <t>과학드림 [Science Dream]</t>
         </is>
       </c>
       <c r="B767" t="inlineStr">
         <is>
-          <t>[음식/요리/레시피]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C767" t="inlineStr">
@@ -21133,24 +21133,24 @@
       </c>
       <c r="D767" t="inlineStr">
         <is>
-          <t>2억0087만</t>
+          <t>1억9880만</t>
         </is>
       </c>
       <c r="E767" t="inlineStr">
         <is>
-          <t>565개</t>
+          <t>148개</t>
         </is>
       </c>
     </row>
     <row r="768">
       <c r="A768" t="inlineStr">
         <is>
-          <t>과학드림 [Science Dream]</t>
+          <t>얌무YAMMoo</t>
         </is>
       </c>
       <c r="B768" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[음식/요리/레시피]</t>
         </is>
       </c>
       <c r="C768" t="inlineStr">
@@ -21160,12 +21160,12 @@
       </c>
       <c r="D768" t="inlineStr">
         <is>
-          <t>1억9855만</t>
+          <t>2억0087만</t>
         </is>
       </c>
       <c r="E768" t="inlineStr">
         <is>
-          <t>148개</t>
+          <t>565개</t>
         </is>
       </c>
     </row>
@@ -21295,7 +21295,7 @@
       </c>
       <c r="D773" t="inlineStr">
         <is>
-          <t>5억4866만</t>
+          <t>5억4868만</t>
         </is>
       </c>
       <c r="E773" t="inlineStr">
@@ -21484,12 +21484,12 @@
       </c>
       <c r="D780" t="inlineStr">
         <is>
-          <t>2억1128만</t>
+          <t>2억1137만</t>
         </is>
       </c>
       <c r="E780" t="inlineStr">
         <is>
-          <t>359개</t>
+          <t>361개</t>
         </is>
       </c>
     </row>
@@ -21712,12 +21712,12 @@
     <row r="789">
       <c r="A789" t="inlineStr">
         <is>
-          <t>LJ Dance</t>
+          <t>칰타</t>
         </is>
       </c>
       <c r="B789" t="inlineStr">
         <is>
-          <t>[음악/댄스/가수]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C789" t="inlineStr">
@@ -21727,24 +21727,24 @@
       </c>
       <c r="D789" t="inlineStr">
         <is>
-          <t>1억6887만</t>
+          <t>2억6753만</t>
         </is>
       </c>
       <c r="E789" t="inlineStr">
         <is>
-          <t>2,902개</t>
+          <t>205개</t>
         </is>
       </c>
     </row>
     <row r="790">
       <c r="A790" t="inlineStr">
         <is>
-          <t>Dorami</t>
+          <t>LJ Dance</t>
         </is>
       </c>
       <c r="B790" t="inlineStr">
         <is>
-          <t>[게임]</t>
+          <t>[음악/댄스/가수]</t>
         </is>
       </c>
       <c r="C790" t="inlineStr">
@@ -21754,24 +21754,24 @@
       </c>
       <c r="D790" t="inlineStr">
         <is>
-          <t>2억4349만</t>
+          <t>1억6887만</t>
         </is>
       </c>
       <c r="E790" t="inlineStr">
         <is>
-          <t>1,212개</t>
+          <t>2,902개</t>
         </is>
       </c>
     </row>
     <row r="791">
       <c r="A791" t="inlineStr">
         <is>
-          <t>배꼽빌라</t>
+          <t>Dorami</t>
         </is>
       </c>
       <c r="B791" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[게임]</t>
         </is>
       </c>
       <c r="C791" t="inlineStr">
@@ -21781,24 +21781,24 @@
       </c>
       <c r="D791" t="inlineStr">
         <is>
-          <t>3억9372만</t>
+          <t>2억4349만</t>
         </is>
       </c>
       <c r="E791" t="inlineStr">
         <is>
-          <t>663개</t>
+          <t>1,212개</t>
         </is>
       </c>
     </row>
     <row r="792">
       <c r="A792" t="inlineStr">
         <is>
-          <t>미미미누</t>
+          <t>배꼽빌라</t>
         </is>
       </c>
       <c r="B792" t="inlineStr">
         <is>
-          <t>[교육/강의]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C792" t="inlineStr">
@@ -21808,24 +21808,24 @@
       </c>
       <c r="D792" t="inlineStr">
         <is>
-          <t>3억9783만</t>
+          <t>3억9372만</t>
         </is>
       </c>
       <c r="E792" t="inlineStr">
         <is>
-          <t>810개</t>
+          <t>663개</t>
         </is>
       </c>
     </row>
     <row r="793">
       <c r="A793" t="inlineStr">
         <is>
-          <t>이라이라경 ravely</t>
+          <t>미미미누</t>
         </is>
       </c>
       <c r="B793" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[교육/강의]</t>
         </is>
       </c>
       <c r="C793" t="inlineStr">
@@ -21835,24 +21835,24 @@
       </c>
       <c r="D793" t="inlineStr">
         <is>
-          <t>4억5908만</t>
+          <t>3억9783만</t>
         </is>
       </c>
       <c r="E793" t="inlineStr">
         <is>
-          <t>605개</t>
+          <t>810개</t>
         </is>
       </c>
     </row>
     <row r="794">
       <c r="A794" t="inlineStr">
         <is>
-          <t>허미노MINO</t>
+          <t>이라이라경 ravely</t>
         </is>
       </c>
       <c r="B794" t="inlineStr">
         <is>
-          <t>[음식/요리/레시피]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C794" t="inlineStr">
@@ -21862,24 +21862,24 @@
       </c>
       <c r="D794" t="inlineStr">
         <is>
-          <t>3억9969만</t>
+          <t>4억5908만</t>
         </is>
       </c>
       <c r="E794" t="inlineStr">
         <is>
-          <t>2,064개</t>
+          <t>605개</t>
         </is>
       </c>
     </row>
     <row r="795">
       <c r="A795" t="inlineStr">
         <is>
-          <t>건나물TV</t>
+          <t>허미노MINO</t>
         </is>
       </c>
       <c r="B795" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[음식/요리/레시피]</t>
         </is>
       </c>
       <c r="C795" t="inlineStr">
@@ -21889,19 +21889,19 @@
       </c>
       <c r="D795" t="inlineStr">
         <is>
-          <t>4억1026만</t>
+          <t>3억9969만</t>
         </is>
       </c>
       <c r="E795" t="inlineStr">
         <is>
-          <t>761개</t>
+          <t>2,064개</t>
         </is>
       </c>
     </row>
     <row r="796">
       <c r="A796" t="inlineStr">
         <is>
-          <t>칰타</t>
+          <t>건나물TV</t>
         </is>
       </c>
       <c r="B796" t="inlineStr">
@@ -21911,17 +21911,17 @@
       </c>
       <c r="C796" t="inlineStr">
         <is>
-          <t>92만</t>
+          <t>93만</t>
         </is>
       </c>
       <c r="D796" t="inlineStr">
         <is>
-          <t>2억6409만</t>
+          <t>4억1026만</t>
         </is>
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>202개</t>
+          <t>761개</t>
         </is>
       </c>
     </row>
@@ -22073,12 +22073,12 @@
       </c>
       <c r="C802" t="inlineStr">
         <is>
-          <t>91만</t>
+          <t>92만</t>
         </is>
       </c>
       <c r="D802" t="inlineStr">
         <is>
-          <t>5억2080만</t>
+          <t>5억2144만</t>
         </is>
       </c>
       <c r="E802" t="inlineStr">
@@ -22441,12 +22441,12 @@
     <row r="816">
       <c r="A816" t="inlineStr">
         <is>
-          <t>소프</t>
+          <t>STUDIO LICO</t>
         </is>
       </c>
       <c r="B816" t="inlineStr">
         <is>
-          <t>[음식/요리/레시피]</t>
+          <t>[영화/만화/애니]</t>
         </is>
       </c>
       <c r="C816" t="inlineStr">
@@ -22456,24 +22456,24 @@
       </c>
       <c r="D816" t="inlineStr">
         <is>
-          <t>3억6301만</t>
+          <t>1억4865만</t>
         </is>
       </c>
       <c r="E816" t="inlineStr">
         <is>
-          <t>1,573개</t>
+          <t>288개</t>
         </is>
       </c>
     </row>
     <row r="817">
       <c r="A817" t="inlineStr">
         <is>
-          <t>STUDIO LICO</t>
+          <t>소프</t>
         </is>
       </c>
       <c r="B817" t="inlineStr">
         <is>
-          <t>[영화/만화/애니]</t>
+          <t>[음식/요리/레시피]</t>
         </is>
       </c>
       <c r="C817" t="inlineStr">
@@ -22483,12 +22483,12 @@
       </c>
       <c r="D817" t="inlineStr">
         <is>
-          <t>1억4838만</t>
+          <t>3억6301만</t>
         </is>
       </c>
       <c r="E817" t="inlineStr">
         <is>
-          <t>287개</t>
+          <t>1,573개</t>
         </is>
       </c>
     </row>
@@ -22630,12 +22630,12 @@
     <row r="823">
       <c r="A823" t="inlineStr">
         <is>
-          <t>815머니톡</t>
+          <t>Soy ASMR</t>
         </is>
       </c>
       <c r="B823" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[취미/라이프]</t>
         </is>
       </c>
       <c r="C823" t="inlineStr">
@@ -22645,19 +22645,19 @@
       </c>
       <c r="D823" t="inlineStr">
         <is>
-          <t>3억5879만</t>
+          <t>1억9957만</t>
         </is>
       </c>
       <c r="E823" t="inlineStr">
         <is>
-          <t>6,245개</t>
+          <t>596개</t>
         </is>
       </c>
     </row>
     <row r="824">
       <c r="A824" t="inlineStr">
         <is>
-          <t>과나gwana</t>
+          <t>815머니톡</t>
         </is>
       </c>
       <c r="B824" t="inlineStr">
@@ -22672,24 +22672,24 @@
       </c>
       <c r="D824" t="inlineStr">
         <is>
-          <t>2억3316만</t>
+          <t>3억5879만</t>
         </is>
       </c>
       <c r="E824" t="inlineStr">
         <is>
-          <t>160개</t>
+          <t>6,245개</t>
         </is>
       </c>
     </row>
     <row r="825">
       <c r="A825" t="inlineStr">
         <is>
-          <t>Soy ASMR</t>
+          <t>과나gwana</t>
         </is>
       </c>
       <c r="B825" t="inlineStr">
         <is>
-          <t>[취미/라이프]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C825" t="inlineStr">
@@ -22699,12 +22699,12 @@
       </c>
       <c r="D825" t="inlineStr">
         <is>
-          <t>1억9939만</t>
+          <t>2억3316만</t>
         </is>
       </c>
       <c r="E825" t="inlineStr">
         <is>
-          <t>596개</t>
+          <t>160개</t>
         </is>
       </c>
     </row>
@@ -22792,39 +22792,39 @@
     <row r="829">
       <c r="A829" t="inlineStr">
         <is>
-          <t>KBS Entertain: 깔깔티비</t>
+          <t>희철리즘Heechulism</t>
         </is>
       </c>
       <c r="B829" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[취미/라이프]</t>
         </is>
       </c>
       <c r="C829" t="inlineStr">
         <is>
-          <t>88만</t>
+          <t>89만</t>
         </is>
       </c>
       <c r="D829" t="inlineStr">
         <is>
-          <t>15억0882만</t>
+          <t>2억2695만</t>
         </is>
       </c>
       <c r="E829" t="inlineStr">
         <is>
-          <t>6,770개</t>
+          <t>344개</t>
         </is>
       </c>
     </row>
     <row r="830">
       <c r="A830" t="inlineStr">
         <is>
-          <t>Dana ASMR</t>
+          <t>KBS Entertain: 깔깔티비</t>
         </is>
       </c>
       <c r="B830" t="inlineStr">
         <is>
-          <t>[취미/라이프]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C830" t="inlineStr">
@@ -22834,19 +22834,19 @@
       </c>
       <c r="D830" t="inlineStr">
         <is>
-          <t>3억1611만</t>
+          <t>15억0882만</t>
         </is>
       </c>
       <c r="E830" t="inlineStr">
         <is>
-          <t>255개</t>
+          <t>6,770개</t>
         </is>
       </c>
     </row>
     <row r="831">
       <c r="A831" t="inlineStr">
         <is>
-          <t>희철리즘Heechulism</t>
+          <t>Dana ASMR</t>
         </is>
       </c>
       <c r="B831" t="inlineStr">
@@ -22861,12 +22861,12 @@
       </c>
       <c r="D831" t="inlineStr">
         <is>
-          <t>2억2632만</t>
+          <t>3억1611만</t>
         </is>
       </c>
       <c r="E831" t="inlineStr">
         <is>
-          <t>343개</t>
+          <t>255개</t>
         </is>
       </c>
     </row>
@@ -23158,7 +23158,7 @@
       </c>
       <c r="D842" t="inlineStr">
         <is>
-          <t>1209만</t>
+          <t>1210만</t>
         </is>
       </c>
       <c r="E842" t="inlineStr">
@@ -23224,12 +23224,12 @@
     <row r="845">
       <c r="A845" t="inlineStr">
         <is>
-          <t>군림보</t>
+          <t>집나간햄지 Wandering Hamzy</t>
         </is>
       </c>
       <c r="B845" t="inlineStr">
         <is>
-          <t>[게임]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C845" t="inlineStr">
@@ -23239,46 +23239,46 @@
       </c>
       <c r="D845" t="inlineStr">
         <is>
-          <t>7억4514만</t>
+          <t>7003만</t>
         </is>
       </c>
       <c r="E845" t="inlineStr">
         <is>
-          <t>5,391개</t>
+          <t>134개</t>
         </is>
       </c>
     </row>
     <row r="846">
       <c r="A846" t="inlineStr">
         <is>
-          <t>차은우 CHAEUNWOO</t>
+          <t>군림보</t>
         </is>
       </c>
       <c r="B846" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[게임]</t>
         </is>
       </c>
       <c r="C846" t="inlineStr">
         <is>
-          <t>86만</t>
+          <t>87만</t>
         </is>
       </c>
       <c r="D846" t="inlineStr">
         <is>
-          <t>1469만</t>
+          <t>7억4514만</t>
         </is>
       </c>
       <c r="E846" t="inlineStr">
         <is>
-          <t>15개</t>
+          <t>5,391개</t>
         </is>
       </c>
     </row>
     <row r="847">
       <c r="A847" t="inlineStr">
         <is>
-          <t>집나간햄지 Wandering Hamzy</t>
+          <t>차은우 CHAEUNWOO</t>
         </is>
       </c>
       <c r="B847" t="inlineStr">
@@ -23293,12 +23293,12 @@
       </c>
       <c r="D847" t="inlineStr">
         <is>
-          <t>6958만</t>
+          <t>1469만</t>
         </is>
       </c>
       <c r="E847" t="inlineStr">
         <is>
-          <t>133개</t>
+          <t>15개</t>
         </is>
       </c>
     </row>
@@ -23482,12 +23482,12 @@
       </c>
       <c r="D854" t="inlineStr">
         <is>
-          <t>3억6251만</t>
+          <t>3억6271만</t>
         </is>
       </c>
       <c r="E854" t="inlineStr">
         <is>
-          <t>352개</t>
+          <t>353개</t>
         </is>
       </c>
     </row>
@@ -23656,12 +23656,12 @@
     <row r="861">
       <c r="A861" t="inlineStr">
         <is>
-          <t>LCK</t>
+          <t>여수MBC Music+(Kpop&amp;Trot)</t>
         </is>
       </c>
       <c r="B861" t="inlineStr">
         <is>
-          <t>[게임]</t>
+          <t>[뉴스/정치/사회]</t>
         </is>
       </c>
       <c r="C861" t="inlineStr">
@@ -23671,51 +23671,51 @@
       </c>
       <c r="D861" t="inlineStr">
         <is>
-          <t>10억6020만</t>
+          <t>5억3563만</t>
         </is>
       </c>
       <c r="E861" t="inlineStr">
         <is>
-          <t>7,265개</t>
+          <t>16,191개</t>
         </is>
       </c>
     </row>
     <row r="862">
       <c r="A862" t="inlineStr">
         <is>
-          <t>HOLLAND</t>
+          <t>LCK</t>
         </is>
       </c>
       <c r="B862" t="inlineStr">
         <is>
-          <t>[음악/댄스/가수]</t>
+          <t>[게임]</t>
         </is>
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>85만</t>
+          <t>86만</t>
         </is>
       </c>
       <c r="D862" t="inlineStr">
         <is>
-          <t>3244만</t>
+          <t>10억6020만</t>
         </is>
       </c>
       <c r="E862" t="inlineStr">
         <is>
-          <t>38개</t>
+          <t>7,265개</t>
         </is>
       </c>
     </row>
     <row r="863">
       <c r="A863" t="inlineStr">
         <is>
-          <t>머독방송</t>
+          <t>HOLLAND</t>
         </is>
       </c>
       <c r="B863" t="inlineStr">
         <is>
-          <t>[게임]</t>
+          <t>[음악/댄스/가수]</t>
         </is>
       </c>
       <c r="C863" t="inlineStr">
@@ -23725,24 +23725,24 @@
       </c>
       <c r="D863" t="inlineStr">
         <is>
-          <t>9억7319만</t>
+          <t>3244만</t>
         </is>
       </c>
       <c r="E863" t="inlineStr">
         <is>
-          <t>11,831개</t>
+          <t>38개</t>
         </is>
       </c>
     </row>
     <row r="864">
       <c r="A864" t="inlineStr">
         <is>
-          <t>여수MBC Music+(Kpop&amp;Trot)</t>
+          <t>머독방송</t>
         </is>
       </c>
       <c r="B864" t="inlineStr">
         <is>
-          <t>[뉴스/정치/사회]</t>
+          <t>[게임]</t>
         </is>
       </c>
       <c r="C864" t="inlineStr">
@@ -23752,24 +23752,24 @@
       </c>
       <c r="D864" t="inlineStr">
         <is>
-          <t>5억3483만</t>
+          <t>9억7319만</t>
         </is>
       </c>
       <c r="E864" t="inlineStr">
         <is>
-          <t>16,174개</t>
+          <t>11,831개</t>
         </is>
       </c>
     </row>
     <row r="865">
       <c r="A865" t="inlineStr">
         <is>
-          <t>울산큰고래 박성주</t>
+          <t>코믹마트</t>
         </is>
       </c>
       <c r="B865" t="inlineStr">
         <is>
-          <t>[게임]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C865" t="inlineStr">
@@ -23779,24 +23779,24 @@
       </c>
       <c r="D865" t="inlineStr">
         <is>
-          <t>7억3985만</t>
+          <t>6억0037만</t>
         </is>
       </c>
       <c r="E865" t="inlineStr">
         <is>
-          <t>3,664개</t>
+          <t>854개</t>
         </is>
       </c>
     </row>
     <row r="866">
       <c r="A866" t="inlineStr">
         <is>
-          <t>코믹마트</t>
+          <t>풍자테레비</t>
         </is>
       </c>
       <c r="B866" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[BJ/인물/연예인]</t>
         </is>
       </c>
       <c r="C866" t="inlineStr">
@@ -23806,24 +23806,24 @@
       </c>
       <c r="D866" t="inlineStr">
         <is>
-          <t>6억0037만</t>
+          <t>3억4601만</t>
         </is>
       </c>
       <c r="E866" t="inlineStr">
         <is>
-          <t>854개</t>
+          <t>1,357개</t>
         </is>
       </c>
     </row>
     <row r="867">
       <c r="A867" t="inlineStr">
         <is>
-          <t>풍자테레비</t>
+          <t>울산큰고래 박성주</t>
         </is>
       </c>
       <c r="B867" t="inlineStr">
         <is>
-          <t>[BJ/인물/연예인]</t>
+          <t>[게임]</t>
         </is>
       </c>
       <c r="C867" t="inlineStr">
@@ -23833,12 +23833,12 @@
       </c>
       <c r="D867" t="inlineStr">
         <is>
-          <t>3억4601만</t>
+          <t>7억4022만</t>
         </is>
       </c>
       <c r="E867" t="inlineStr">
         <is>
-          <t>1,357개</t>
+          <t>3,665개</t>
         </is>
       </c>
     </row>
@@ -24157,12 +24157,12 @@
       </c>
       <c r="D879" t="inlineStr">
         <is>
-          <t>3억5712만</t>
+          <t>3억5723만</t>
         </is>
       </c>
       <c r="E879" t="inlineStr">
         <is>
-          <t>2,063개</t>
+          <t>2,066개</t>
         </is>
       </c>
     </row>
@@ -24292,7 +24292,7 @@
       </c>
       <c r="D884" t="inlineStr">
         <is>
-          <t>4억2102만</t>
+          <t>4억2229만</t>
         </is>
       </c>
       <c r="E884" t="inlineStr">
@@ -24778,7 +24778,7 @@
       </c>
       <c r="D902" t="inlineStr">
         <is>
-          <t>1억2056만</t>
+          <t>1억2062만</t>
         </is>
       </c>
       <c r="E902" t="inlineStr">
@@ -24859,12 +24859,12 @@
       </c>
       <c r="D905" t="inlineStr">
         <is>
-          <t>2억4813만</t>
+          <t>2억4847만</t>
         </is>
       </c>
       <c r="E905" t="inlineStr">
         <is>
-          <t>1,514개</t>
+          <t>1,515개</t>
         </is>
       </c>
     </row>
@@ -25222,39 +25222,39 @@
     <row r="919">
       <c r="A919" t="inlineStr">
         <is>
-          <t>연다</t>
+          <t>청정구역</t>
         </is>
       </c>
       <c r="B919" t="inlineStr">
         <is>
-          <t>[게임]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C919" t="inlineStr">
         <is>
-          <t>81만</t>
+          <t>80만</t>
         </is>
       </c>
       <c r="D919" t="inlineStr">
         <is>
-          <t>6억3856만</t>
+          <t>4억0105만</t>
         </is>
       </c>
       <c r="E919" t="inlineStr">
         <is>
-          <t>2,366개</t>
+          <t>978개</t>
         </is>
       </c>
     </row>
     <row r="920">
       <c r="A920" t="inlineStr">
         <is>
-          <t>청정구역</t>
+          <t>트래블튜브</t>
         </is>
       </c>
       <c r="B920" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C920" t="inlineStr">
@@ -25264,24 +25264,24 @@
       </c>
       <c r="D920" t="inlineStr">
         <is>
-          <t>4억0105만</t>
+          <t>7억0596만</t>
         </is>
       </c>
       <c r="E920" t="inlineStr">
         <is>
-          <t>978개</t>
+          <t>1,507개</t>
         </is>
       </c>
     </row>
     <row r="921">
       <c r="A921" t="inlineStr">
         <is>
-          <t>트래블튜브</t>
+          <t>연다</t>
         </is>
       </c>
       <c r="B921" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[게임]</t>
         </is>
       </c>
       <c r="C921" t="inlineStr">
@@ -25291,12 +25291,12 @@
       </c>
       <c r="D921" t="inlineStr">
         <is>
-          <t>7억0596만</t>
+          <t>6억3862만</t>
         </is>
       </c>
       <c r="E921" t="inlineStr">
         <is>
-          <t>1,507개</t>
+          <t>2,366개</t>
         </is>
       </c>
     </row>
@@ -25372,7 +25372,7 @@
       </c>
       <c r="D924" t="inlineStr">
         <is>
-          <t>7839만</t>
+          <t>7842만</t>
         </is>
       </c>
       <c r="E924" t="inlineStr">
@@ -26884,7 +26884,7 @@
       </c>
       <c r="D980" t="inlineStr">
         <is>
-          <t>1억3856만</t>
+          <t>1억3875만</t>
         </is>
       </c>
       <c r="E980" t="inlineStr">
@@ -27112,12 +27112,12 @@
     <row r="989">
       <c r="A989" t="inlineStr">
         <is>
-          <t>MBC 미스터리 : 심야괴담회 X 서프라이즈</t>
+          <t>바라던 바다</t>
         </is>
       </c>
       <c r="B989" t="inlineStr">
         <is>
-          <t>[TV/방송]</t>
+          <t>[미분류]</t>
         </is>
       </c>
       <c r="C989" t="inlineStr">
@@ -27127,24 +27127,24 @@
       </c>
       <c r="D989" t="inlineStr">
         <is>
-          <t>4억0958만</t>
+          <t>3억9476만</t>
         </is>
       </c>
       <c r="E989" t="inlineStr">
         <is>
-          <t>2,875개</t>
+          <t>519개</t>
         </is>
       </c>
     </row>
     <row r="990">
       <c r="A990" t="inlineStr">
         <is>
-          <t>아옳이</t>
+          <t>MBC 미스터리 : 심야괴담회 X 서프라이즈</t>
         </is>
       </c>
       <c r="B990" t="inlineStr">
         <is>
-          <t>[패션/미용]</t>
+          <t>[TV/방송]</t>
         </is>
       </c>
       <c r="C990" t="inlineStr">
@@ -27154,24 +27154,24 @@
       </c>
       <c r="D990" t="inlineStr">
         <is>
-          <t>9520만</t>
+          <t>4억1033만</t>
         </is>
       </c>
       <c r="E990" t="inlineStr">
         <is>
-          <t>136개</t>
+          <t>2,885개</t>
         </is>
       </c>
     </row>
     <row r="991">
       <c r="A991" t="inlineStr">
         <is>
-          <t>바라던 바다</t>
+          <t>아옳이</t>
         </is>
       </c>
       <c r="B991" t="inlineStr">
         <is>
-          <t>[미분류]</t>
+          <t>[패션/미용]</t>
         </is>
       </c>
       <c r="C991" t="inlineStr">
@@ -27181,12 +27181,12 @@
       </c>
       <c r="D991" t="inlineStr">
         <is>
-          <t>3억9408만</t>
+          <t>9520만</t>
         </is>
       </c>
       <c r="E991" t="inlineStr">
         <is>
-          <t>519개</t>
+          <t>136개</t>
         </is>
       </c>
     </row>
@@ -27316,12 +27316,12 @@
       </c>
       <c r="D996" t="inlineStr">
         <is>
-          <t>3억0890만</t>
+          <t>3억0955만</t>
         </is>
       </c>
       <c r="E996" t="inlineStr">
         <is>
-          <t>449개</t>
+          <t>450개</t>
         </is>
       </c>
     </row>

</xml_diff>